<commit_message>
continued working on cross-os framework stability
</commit_message>
<xml_diff>
--- a/src/test/resources/googleApi/dataProviders/DistanceMatrix.xlsx
+++ b/src/test/resources/googleApi/dataProviders/DistanceMatrix.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>TestScenario</t>
   </si>
@@ -37,15 +37,9 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>bicycling</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
-    <t>fr-FR</t>
-  </si>
-  <si>
     <t>API_KEY</t>
   </si>
   <si>
@@ -55,15 +49,9 @@
     <t>ValidateOriginAddress</t>
   </si>
   <si>
-    <t>Vancouver, BC, Canada;Seattle, Washington, Ã‰tats-Unis</t>
-  </si>
-  <si>
     <t>ValidateDestinationAddress</t>
   </si>
   <si>
-    <t>San Francisco, Californie, Ã‰tats-Unis;Victoria, BC, Canada</t>
-  </si>
-  <si>
     <t>en-EN</t>
   </si>
   <si>
@@ -83,18 +71,6 @@
   </si>
   <si>
     <t>json</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>windows</t>
-  </si>
-  <si>
-    <t>mac</t>
-  </si>
-  <si>
-    <t>San Francisco, Californie, États-Unis;Victoria, BC, Canada</t>
   </si>
 </sst>
 </file>
@@ -923,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +917,7 @@
     <col min="8" max="8" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -955,25 +931,22 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -984,28 +957,25 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1016,217 +986,22 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>